<commit_message>
working first DEMO : 7inch Touch Screen + STM32F429ZI
</commit_message>
<xml_diff>
--- a/IHM-PC/program/stm32f429ZI/TouchGFX/assets/texts/texts.xlsx
+++ b/IHM-PC/program/stm32f429ZI/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="48">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -143,51 +143,22 @@
     <t xml:space="preserve">Small</t>
   </si>
   <si>
-    <t xml:space="preserve">Typography_00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GOUDYSTO.TTF</t>
+    <t xml:space="preserve">SingleUseId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">HELLO WORLD !</t>
   </si>
   <si>
     <t xml:space="preserve">SingleUseId2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Left</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LTR</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">HELLO WORLD ON SCREEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MATURASC.TTF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"HELLO WORLD !"
-Not on the console this time :D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"HELLO WORLD !"
-Not on the console this time :D</t>
   </si>
 </sst>
 </file>
@@ -1518,25 +1489,6 @@
       <c r="P6" s="10"/>
     </row>
     <row r="7" spans="2:16">
-      <c r="B7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7">
-        <v>20</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7"/>
       <c r="L7" s="7" t="s">
         <v>7</v>
       </c>
@@ -1669,24 +1621,38 @@
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
         <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s">
         <v>46</v>
       </c>
-      <c r="F4" t="s">
-        <v>56</v>
-      </c>
     </row>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>